<commit_message>
Fix tactic grouping: merge multi-audience rows into single tactics
</commit_message>
<xml_diff>
--- a/public/templates/unilever-traffic-sheet-template.xlsx
+++ b/public/templates/unilever-traffic-sheet-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucusdato/Documents/Dev/ShortStaffed MediaTools/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5BFCB3-6975-8842-AB2A-BC68DF47CB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F26E1-EE5E-F347-B262-9A1EB92BF87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brand Say Digital" sheetId="24" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t xml:space="preserve">INI Activation Programmatic Campaign Brief Information </t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>Live Date</t>
-  </si>
-  <si>
-    <t>Campaign Total Budget</t>
   </si>
   <si>
     <t>Ad Name (Taxonomy from Accutics)</t>
@@ -979,7 +976,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1009,7 +1006,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1220,6 +1216,33 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1234,6 +1257,15 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1258,42 +1290,6 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Currency 2" xfId="13" xr:uid="{8CF7D383-AFB8-449D-BDBA-1A9E198FD9F1}"/>
@@ -1590,625 +1586,625 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="80.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="87.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="31" customWidth="1"/>
-    <col min="16" max="16" width="131.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="220" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="80.7109375" style="31"/>
+    <col min="1" max="1" width="1.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="107.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="30" customWidth="1"/>
+    <col min="16" max="16" width="131.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="220" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="80.7109375" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
     </row>
     <row r="2" spans="1:21" ht="22">
-      <c r="A2" s="30"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="1:21" ht="19">
-      <c r="A3" s="30"/>
-      <c r="B3" s="33" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
+      <c r="C3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21" ht="19">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="1:21" ht="19">
-      <c r="A5" s="36"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
+      <c r="C5" s="39"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
     </row>
     <row r="6" spans="1:21" ht="19">
-      <c r="A6" s="36"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
+      <c r="C6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
     </row>
     <row r="7" spans="1:21" ht="19">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
     </row>
     <row r="8" spans="1:21" ht="19">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="79" t="s">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="R8" s="80"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
     </row>
     <row r="9" spans="1:21" ht="18" customHeight="1">
-      <c r="A9" s="77"/>
-      <c r="B9" s="78" t="s">
+      <c r="A9" s="76"/>
+      <c r="B9" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="45" t="s">
+      <c r="G9" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="78" t="s">
+      <c r="I9" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="78" t="s">
+      <c r="J9" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="78" t="s">
+      <c r="L9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="78" t="s">
+      <c r="M9" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="78" t="s">
+      <c r="N9" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="78" t="s">
+      <c r="O9" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" s="100" t="s">
+      <c r="Q9" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="100" t="s">
+      <c r="R9" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="100" t="s">
+      <c r="S9" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
+      <c r="T9" s="72"/>
+      <c r="U9" s="72"/>
     </row>
     <row r="10" spans="1:21" ht="19">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="103"/>
-      <c r="N10" s="103"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="105"/>
-      <c r="S10" s="105"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="104"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
     </row>
     <row r="11" spans="1:21" ht="19">
-      <c r="A11" s="36"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="108"/>
-      <c r="R11" s="107"/>
-      <c r="S11" s="107"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="105"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
     </row>
     <row r="12" spans="1:21" ht="19">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
     </row>
     <row r="13" spans="1:21" ht="19">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
     </row>
     <row r="14" spans="1:21" ht="19">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
     </row>
     <row r="15" spans="1:21" ht="19">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
     </row>
     <row r="16" spans="1:21" ht="19">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
     </row>
     <row r="17" spans="1:21" ht="16">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
     </row>
     <row r="18" spans="1:21" ht="16">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
     </row>
     <row r="19" spans="1:21" ht="16">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
     </row>
     <row r="20" spans="1:21" ht="16">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
     </row>
     <row r="21" spans="1:21" ht="16">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="30"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
     </row>
     <row r="22" spans="1:21" ht="16">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
     </row>
     <row r="23" spans="1:21" ht="16">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
     </row>
     <row r="24" spans="1:21" ht="16">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2222,400 +2218,400 @@
   </sheetPr>
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" style="31"/>
-    <col min="2" max="2" width="17.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4" style="31" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" style="31"/>
-    <col min="28" max="28" width="10.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9" style="31"/>
+    <col min="1" max="1" width="9" style="30"/>
+    <col min="2" max="2" width="17.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" style="30"/>
+    <col min="28" max="28" width="10.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="16">
-      <c r="A1" s="30"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50" t="s">
+      <c r="A1" s="29"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
     </row>
     <row r="2" spans="1:28" ht="16">
-      <c r="A2" s="30"/>
-      <c r="B2" s="53" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="55" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="57" t="s">
+      <c r="I2" s="48"/>
+      <c r="J2" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
     </row>
     <row r="3" spans="1:28" ht="16">
-      <c r="A3" s="30"/>
-      <c r="B3" s="53" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="59" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="57" t="s">
+      <c r="I3" s="48"/>
+      <c r="J3" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="52"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
     </row>
     <row r="4" spans="1:28" ht="16">
-      <c r="A4" s="30"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="61" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="57" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="49"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
     </row>
     <row r="5" spans="1:28" ht="16">
-      <c r="A5" s="30"/>
-      <c r="B5" s="53" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="64" t="s">
+      <c r="C5" s="59"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="57" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="52"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="49"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
     </row>
     <row r="6" spans="1:28" ht="16">
-      <c r="A6" s="30"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="65" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="57" t="s">
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="57" t="s">
+      <c r="K6" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="52"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="49"/>
-      <c r="X6" s="49"/>
-      <c r="Y6" s="49"/>
-      <c r="Z6" s="49"/>
-      <c r="AA6" s="49"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
     </row>
     <row r="7" spans="1:28" ht="16">
-      <c r="A7" s="30"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="49"/>
-      <c r="Z7" s="49"/>
-      <c r="AA7" s="49"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="48"/>
     </row>
     <row r="8" spans="1:28" ht="16">
-      <c r="A8" s="30"/>
-      <c r="B8" s="68" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="68" t="s">
+      <c r="H8" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="68" t="s">
+      <c r="K8" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="68" t="s">
+      <c r="L8" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="68" t="s">
+      <c r="M8" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="67" t="s">
+      <c r="N8" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="O8" s="67" t="s">
+      <c r="O8" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="67" t="s">
+      <c r="P8" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" s="67" t="s">
+      <c r="Q8" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="67" t="s">
+      <c r="R8" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="S8" s="68" t="s">
+      <c r="S8" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="T8" s="95" t="s">
+      <c r="T8" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="U8" s="68" t="s">
+      <c r="U8" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="V8" s="68" t="s">
+      <c r="V8" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="W8" s="68" t="s">
+      <c r="W8" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="X8" s="68" t="s">
+      <c r="X8" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="68" t="s">
+      <c r="Y8" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="Z8" s="95" t="s">
+      <c r="Z8" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="AA8" s="49"/>
+      <c r="AA8" s="48"/>
     </row>
     <row r="9" spans="1:28" ht="16" customHeight="1">
-      <c r="A9" s="83"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="97"/>
-      <c r="T9" s="89"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="87"/>
-      <c r="X9" s="88"/>
-      <c r="Y9" s="88"/>
-      <c r="Z9" s="86"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="93"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="91"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="84"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="95"/>
+      <c r="S9" s="96"/>
+      <c r="T9" s="88"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="85"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="85"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="92"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:28" ht="15" customHeight="1"/>
@@ -2632,39 +2628,40 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16">
+    <row r="1" spans="1:25" ht="16">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2672,14 +2669,14 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="112" t="s">
+      <c r="I1" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="113"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -2694,37 +2691,36 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="16">
+    </row>
+    <row r="2" spans="1:25" ht="16">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5" t="s">
         <v>24</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="114" t="s">
+      <c r="I2" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="115"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -2734,37 +2730,36 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="16">
+    </row>
+    <row r="3" spans="1:25" ht="16">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="114" t="s">
+      <c r="I3" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="115"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -2774,33 +2769,32 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" ht="16">
+    </row>
+    <row r="4" spans="1:25" ht="16">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="9" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="9" t="s">
         <v>34</v>
       </c>
+      <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="114" t="s">
+      <c r="I4" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="115"/>
-      <c r="L4" s="116"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -2810,33 +2804,32 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" ht="16">
+    </row>
+    <row r="5" spans="1:25" ht="16">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="12" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="12" t="s">
         <v>38</v>
       </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -2846,31 +2839,30 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" ht="16">
+    </row>
+    <row r="6" spans="1:25" ht="16">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="16" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="15" t="s">
         <v>41</v>
       </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="I6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -2880,25 +2872,24 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" ht="16">
+    </row>
+    <row r="7" spans="1:25" ht="16">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -2908,119 +2899,114 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" ht="16">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
+    </row>
+    <row r="8" spans="1:25" ht="16">
+      <c r="A8" s="20"/>
+      <c r="B8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="O8" s="19" t="s">
+      <c r="N8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="O8" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="P8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="R8" s="18" t="s">
+      <c r="Q8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="R8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="T8" s="18" t="s">
+      <c r="S8" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="U8" s="18" t="s">
+      <c r="T8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="V8" s="18" t="s">
+      <c r="U8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="18" t="s">
+      <c r="V8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="W8" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="Y8" s="20" t="s">
+      <c r="X8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" s="139" customFormat="1" ht="16">
-      <c r="A9" s="129"/>
-      <c r="B9" s="130"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="134"/>
-      <c r="M9" s="135"/>
-      <c r="N9" s="135"/>
-      <c r="O9" s="135"/>
-      <c r="P9" s="134"/>
-      <c r="Q9" s="134"/>
-      <c r="R9" s="136"/>
-      <c r="S9" s="136"/>
-      <c r="T9" s="136"/>
-      <c r="U9" s="137"/>
-      <c r="V9" s="136"/>
-      <c r="W9" s="136"/>
-      <c r="X9" s="136"/>
-      <c r="Y9" s="137"/>
-      <c r="Z9" s="138"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" s="121" customFormat="1" ht="16">
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="117"/>
+      <c r="M9" s="117"/>
+      <c r="N9" s="117"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="116"/>
+      <c r="Q9" s="118"/>
+      <c r="R9" s="118"/>
+      <c r="S9" s="118"/>
+      <c r="T9" s="119"/>
+      <c r="U9" s="118"/>
+      <c r="V9" s="118"/>
+      <c r="W9" s="118"/>
+      <c r="X9" s="119"/>
+      <c r="Y9" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3052,366 +3038,361 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="22"/>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
-      <c r="A3" s="22"/>
-      <c r="B3" s="109" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="126"/>
-      <c r="B4" s="127" t="s">
+      <c r="A4" s="128"/>
+      <c r="B4" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="127" t="s">
+      <c r="C4" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="127" t="s">
+      <c r="D4" s="129" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="127" t="s">
+      <c r="E4" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="124" t="s">
+      <c r="F4" s="137" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="118" t="s">
+      <c r="H4" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="I4" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="131" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="133"/>
+      <c r="L4" s="134"/>
+    </row>
+    <row r="5" spans="1:12" ht="16">
+      <c r="A5" s="128"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I5" s="132"/>
+      <c r="J5" s="132"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="134"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="21"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="21"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="21"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="21"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="21"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="21"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="21"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1">
+      <c r="A14" s="21"/>
+      <c r="B14" s="108" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" ht="16">
+      <c r="A15" s="22"/>
+      <c r="B15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="L15" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="120"/>
-      <c r="L4" s="121"/>
-    </row>
-    <row r="5" spans="1:12" ht="16">
-      <c r="A5" s="126"/>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="121"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="22"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="22"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="22"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="22"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="22"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="22"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="22"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="109" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-    </row>
-    <row r="15" spans="1:12" ht="16">
-      <c r="A15" s="23"/>
-      <c r="B15" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="29" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="22"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="22"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="22"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="22"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="22"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
@@ -3420,6 +3401,11 @@
     <mergeCell ref="F1:H3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3448,45 +3434,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="D1" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="E1" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="F1" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="G1" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="75" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:7" ht="239.25" customHeight="1">
-      <c r="A3" s="71"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3494,6 +3480,40 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9">
+      <UserInfo>
+        <DisplayName>Michell, Matthew (TOR-KSO)</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Varghis, Elizabeth (TOR-INI)</DisplayName>
+        <AccountId>2025</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MediaLengthInSeconds xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E378BB92EEB2A145A79C64826753F547" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9b1b7f9f89fc98b6bebad2deac5d96e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xmlns:ns3="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8043f776218cda17cbf8603499f1ce26" ns2:_="" ns3:_="">
     <xsd:import namespace="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
@@ -3740,41 +3760,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3541FD-1447-4F7B-AFA2-CC6EF8E7740D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9"/>
+    <ds:schemaRef ds:uri="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9">
-      <UserInfo>
-        <DisplayName>Michell, Matthew (TOR-KSO)</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Varghis, Elizabeth (TOR-INI)</DisplayName>
-        <AccountId>2025</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MediaLengthInSeconds xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F18C043-8739-45D3-BBF5-921B1C89D4FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ABDA3BC-60BE-4BA1-BF3C-336860CC5BED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3793,25 +3798,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F18C043-8739-45D3-BBF5-921B1C89D4FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3541FD-1447-4F7B-AFA2-CC6EF8E7740D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9"/>
-    <ds:schemaRef ds:uri="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d026e4c1-5892-497a-b9da-ee493c9f0364}" enabled="0" method="" siteId="{d026e4c1-5892-497a-b9da-ee493c9f0364}" removed="1"/>

</xml_diff>

<commit_message>
✨ Improve excluded row handling and reorganize campaign fields
- Show excluded rows (OOH, TV, Radio, Print) in verification screen with red styling
- Restrict CSV download button to admin users only
- Move Buy Type and Ad Set Budget fields to campaign level (from ad group level)
- Update Brand Say Digital border config to include YouTube columns (G-U instead of G-S)
- Enhance categorization to detect excluded channels by keywords directly
- Update traffic sheet template with new field organization

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/unilever-traffic-sheet-template.xlsx
+++ b/public/templates/unilever-traffic-sheet-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucusdato/Documents/Dev/ShortStaffed MediaTools/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC9903-312B-4C47-9EE6-917BD3571151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1C3166-4EE2-2147-BDFA-9CDEC7DC0445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="87">
   <si>
     <t xml:space="preserve">INI Activation Programmatic Campaign Brief Information </t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>Audience size in FR</t>
+  </si>
+  <si>
+    <t>CALL TO ACTION (10)</t>
+  </si>
+  <si>
+    <t>HEADLINE (70)</t>
   </si>
 </sst>
 </file>
@@ -1239,6 +1245,15 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1261,15 +1276,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1560,10 +1566,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="80.7109375" defaultRowHeight="15"/>
@@ -1587,10 +1593,12 @@
     <col min="17" max="17" width="17.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.28515625" style="30" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="80.7109375" style="30"/>
+    <col min="20" max="20" width="25.85546875" style="30" customWidth="1"/>
+    <col min="21" max="21" width="39.42578125" style="30" customWidth="1"/>
+    <col min="22" max="16384" width="80.7109375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16">
+    <row r="1" spans="1:22" ht="16">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -1612,8 +1620,9 @@
       <c r="S1" s="29"/>
       <c r="T1" s="29"/>
       <c r="U1" s="29"/>
-    </row>
-    <row r="2" spans="1:21" ht="22">
+      <c r="V1" s="29"/>
+    </row>
+    <row r="2" spans="1:22" ht="22">
       <c r="A2" s="29"/>
       <c r="B2" s="31" t="s">
         <v>0</v>
@@ -1636,8 +1645,9 @@
       <c r="S2" s="29"/>
       <c r="T2" s="29"/>
       <c r="U2" s="29"/>
-    </row>
-    <row r="3" spans="1:21" ht="19">
+      <c r="V2" s="29"/>
+    </row>
+    <row r="3" spans="1:22" ht="19">
       <c r="A3" s="29"/>
       <c r="B3" s="32" t="s">
         <v>1</v>
@@ -1659,8 +1669,9 @@
       <c r="S3" s="29"/>
       <c r="T3" s="29"/>
       <c r="U3" s="29"/>
-    </row>
-    <row r="4" spans="1:21" ht="19">
+      <c r="V3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" ht="19">
       <c r="A4" s="35"/>
       <c r="B4" s="36" t="s">
         <v>2</v>
@@ -1683,8 +1694,9 @@
       <c r="S4" s="35"/>
       <c r="T4" s="35"/>
       <c r="U4" s="35"/>
-    </row>
-    <row r="5" spans="1:21" ht="19">
+      <c r="V4" s="35"/>
+    </row>
+    <row r="5" spans="1:22" ht="19">
       <c r="A5" s="35"/>
       <c r="B5" s="38" t="s">
         <v>3</v>
@@ -1707,8 +1719,9 @@
       <c r="S5" s="35"/>
       <c r="T5" s="35"/>
       <c r="U5" s="35"/>
-    </row>
-    <row r="6" spans="1:21" ht="19">
+      <c r="V5" s="35"/>
+    </row>
+    <row r="6" spans="1:22" ht="19">
       <c r="A6" s="35"/>
       <c r="B6" s="38" t="s">
         <v>4</v>
@@ -1731,8 +1744,9 @@
       <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="35"/>
-    </row>
-    <row r="7" spans="1:21" ht="19">
+      <c r="V6" s="35"/>
+    </row>
+    <row r="7" spans="1:22" ht="19">
       <c r="A7" s="43"/>
       <c r="B7" s="43"/>
       <c r="C7" s="41"/>
@@ -1754,10 +1768,11 @@
       </c>
       <c r="R7" s="79"/>
       <c r="S7" s="42"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-    </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1">
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="43"/>
+    </row>
+    <row r="8" spans="1:22" ht="18" customHeight="1">
       <c r="A8" s="76"/>
       <c r="B8" s="77" t="s">
         <v>6</v>
@@ -1813,10 +1828,15 @@
       <c r="S8" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72"/>
-    </row>
-    <row r="9" spans="1:21" ht="19">
+      <c r="T8" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="U8" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="V8" s="72"/>
+    </row>
+    <row r="9" spans="1:22" ht="19">
       <c r="A9" s="45" t="s">
         <v>21</v>
       </c>
@@ -1838,10 +1858,11 @@
       <c r="Q9" s="103"/>
       <c r="R9" s="104"/>
       <c r="S9" s="104"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-    </row>
-    <row r="10" spans="1:21" ht="19">
+      <c r="T9" s="104"/>
+      <c r="U9" s="104"/>
+      <c r="V9" s="29"/>
+    </row>
+    <row r="10" spans="1:22" ht="19">
       <c r="A10" s="35"/>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -1861,10 +1882,11 @@
       <c r="Q10" s="35"/>
       <c r="R10" s="35"/>
       <c r="S10" s="35"/>
-      <c r="T10" s="29"/>
+      <c r="T10" s="35"/>
       <c r="U10" s="29"/>
-    </row>
-    <row r="11" spans="1:21" ht="19">
+      <c r="V10" s="29"/>
+    </row>
+    <row r="11" spans="1:22" ht="19">
       <c r="A11" s="35"/>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
@@ -1884,10 +1906,11 @@
       <c r="Q11" s="35"/>
       <c r="R11" s="35"/>
       <c r="S11" s="35"/>
-      <c r="T11" s="29"/>
+      <c r="T11" s="35"/>
       <c r="U11" s="29"/>
-    </row>
-    <row r="12" spans="1:21" ht="19">
+      <c r="V11" s="29"/>
+    </row>
+    <row r="12" spans="1:22" ht="19">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -1909,10 +1932,11 @@
       <c r="Q12" s="35"/>
       <c r="R12" s="35"/>
       <c r="S12" s="35"/>
-      <c r="T12" s="29"/>
+      <c r="T12" s="35"/>
       <c r="U12" s="29"/>
-    </row>
-    <row r="13" spans="1:21" ht="19">
+      <c r="V12" s="29"/>
+    </row>
+    <row r="13" spans="1:22" ht="19">
       <c r="A13" s="35"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -1932,10 +1956,11 @@
       <c r="Q13" s="35"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
-      <c r="T13" s="29"/>
+      <c r="T13" s="35"/>
       <c r="U13" s="29"/>
-    </row>
-    <row r="14" spans="1:21" ht="19">
+      <c r="V13" s="29"/>
+    </row>
+    <row r="14" spans="1:22" ht="19">
       <c r="A14" s="35"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -1955,10 +1980,11 @@
       <c r="Q14" s="35"/>
       <c r="R14" s="35"/>
       <c r="S14" s="35"/>
-      <c r="T14" s="29"/>
+      <c r="T14" s="35"/>
       <c r="U14" s="29"/>
-    </row>
-    <row r="15" spans="1:21" ht="16">
+      <c r="V14" s="29"/>
+    </row>
+    <row r="15" spans="1:22" ht="16">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -1980,8 +2006,9 @@
       <c r="S15" s="29"/>
       <c r="T15" s="29"/>
       <c r="U15" s="29"/>
-    </row>
-    <row r="16" spans="1:21" ht="16">
+      <c r="V15" s="29"/>
+    </row>
+    <row r="16" spans="1:22" ht="16">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -2003,8 +2030,9 @@
       <c r="S16" s="29"/>
       <c r="T16" s="29"/>
       <c r="U16" s="29"/>
-    </row>
-    <row r="17" spans="1:21" ht="16">
+      <c r="V16" s="29"/>
+    </row>
+    <row r="17" spans="1:22" ht="16">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -2026,8 +2054,9 @@
       <c r="S17" s="29"/>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
-    </row>
-    <row r="18" spans="1:21" ht="16">
+      <c r="V17" s="29"/>
+    </row>
+    <row r="18" spans="1:22" ht="16">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -2049,8 +2078,9 @@
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
       <c r="U18" s="29"/>
-    </row>
-    <row r="19" spans="1:21" ht="16">
+      <c r="V18" s="29"/>
+    </row>
+    <row r="19" spans="1:22" ht="16">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -2072,8 +2102,9 @@
       <c r="S19" s="29"/>
       <c r="T19" s="29"/>
       <c r="U19" s="29"/>
-    </row>
-    <row r="20" spans="1:21" ht="16">
+      <c r="V19" s="29"/>
+    </row>
+    <row r="20" spans="1:22" ht="16">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -2095,8 +2126,9 @@
       <c r="S20" s="29"/>
       <c r="T20" s="29"/>
       <c r="U20" s="29"/>
-    </row>
-    <row r="21" spans="1:21" ht="16">
+      <c r="V20" s="29"/>
+    </row>
+    <row r="21" spans="1:22" ht="16">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -2118,8 +2150,9 @@
       <c r="S21" s="29"/>
       <c r="T21" s="29"/>
       <c r="U21" s="29"/>
-    </row>
-    <row r="22" spans="1:21" ht="16">
+      <c r="V21" s="29"/>
+    </row>
+    <row r="22" spans="1:22" ht="16">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="47"/>
@@ -2141,6 +2174,7 @@
       <c r="S22" s="29"/>
       <c r="T22" s="29"/>
       <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2975,13 +3009,13 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="21"/>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
@@ -2993,9 +3027,9 @@
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
@@ -3009,61 +3043,61 @@
       <c r="C3" s="106"/>
       <c r="D3" s="106"/>
       <c r="E3" s="107"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
     </row>
     <row r="4" spans="1:12" ht="16">
-      <c r="A4" s="133"/>
-      <c r="B4" s="134" t="s">
+      <c r="A4" s="125"/>
+      <c r="B4" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="126" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="134" t="s">
+      <c r="D4" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="134" t="s">
+      <c r="E4" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="131" t="s">
+      <c r="F4" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="125" t="s">
+      <c r="G4" s="128" t="s">
         <v>72</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="125" t="s">
+      <c r="I4" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="125" t="s">
+      <c r="J4" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="127"/>
-      <c r="L4" s="128"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="131"/>
     </row>
     <row r="5" spans="1:12" ht="16">
-      <c r="A5" s="133"/>
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="126"/>
+      <c r="A5" s="125"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="129"/>
       <c r="H5" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="128"/>
+      <c r="I5" s="129"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="131"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="21"/>
@@ -3329,11 +3363,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
@@ -3342,6 +3371,11 @@
     <mergeCell ref="F1:H3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3416,6 +3450,40 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9">
+      <UserInfo>
+        <DisplayName>Michell, Matthew (TOR-KSO)</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Varghis, Elizabeth (TOR-INI)</DisplayName>
+        <AccountId>2025</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MediaLengthInSeconds xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E378BB92EEB2A145A79C64826753F547" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9b1b7f9f89fc98b6bebad2deac5d96e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xmlns:ns3="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8043f776218cda17cbf8603499f1ce26" ns2:_="" ns3:_="">
     <xsd:import namespace="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
@@ -3662,41 +3730,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3541FD-1447-4F7B-AFA2-CC6EF8E7740D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9"/>
+    <ds:schemaRef ds:uri="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9">
-      <UserInfo>
-        <DisplayName>Michell, Matthew (TOR-KSO)</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Varghis, Elizabeth (TOR-INI)</DisplayName>
-        <AccountId>2025</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MediaLengthInSeconds xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F18C043-8739-45D3-BBF5-921B1C89D4FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ABDA3BC-60BE-4BA1-BF3C-336860CC5BED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3715,25 +3768,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F18C043-8739-45D3-BBF5-921B1C89D4FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C3541FD-1447-4F7B-AFA2-CC6EF8E7740D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f065b57-ebdc-4f10-a6ee-7426bc8f4fe9"/>
-    <ds:schemaRef ds:uri="c8231cc5-c9e0-4ca6-8c96-bdc0cfec0c86"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d026e4c1-5892-497a-b9da-ee493c9f0364}" enabled="0" method="" siteId="{d026e4c1-5892-497a-b9da-ee493c9f0364}" removed="1"/>

</xml_diff>